<commit_message>
Changes in roles and naming convention
</commit_message>
<xml_diff>
--- a/data/aad/Rollen.xlsx
+++ b/data/aad/Rollen.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9CE00E-75A1-4B1C-9E63-FEF7D2A93FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4258576-6CE4-4F34-A625-738C520F1B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="4188" windowWidth="29208" windowHeight="12024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setupRoles" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="105">
   <si>
     <t>Role</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>Insights Analyst</t>
+  </si>
+  <si>
+    <t>Yammer Administrator</t>
+  </si>
+  <si>
+    <t>Lifecycle Workflows Administrator</t>
+  </si>
+  <si>
+    <t>Permissions Management Administrator</t>
   </si>
 </sst>
 </file>
@@ -726,7 +735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -906,12 +917,18 @@
         <v>94</v>
       </c>
       <c r="B17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
@@ -1510,23 +1527,29 @@
       <c r="B92" s="4"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="2"/>
+      <c r="A93" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="2"/>
+      <c r="A94" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
+      <c r="A95" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="2"/>
+      <c r="A96" s="5"/>
       <c r="B96" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:A97">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:A96">
     <sortCondition ref="A8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>